<commit_message>
functionality: option to convert to .mov
</commit_message>
<xml_diff>
--- a/conversion/conversion_log.xlsx
+++ b/conversion/conversion_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,6 +505,174 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/abcd.R3D</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/abcd.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/A008_B009_1025IF_001.R3D</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/A008_B009_1025IF_001.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/d2 copy/efgh.R3D</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/d2 copy/efgh.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/abcd.R3D</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/abcd.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/A008_B009_1025IF_001.R3D</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/A008_B009_1025IF_001.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/d2 copy/efgh.R3D</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/d2 copy/efgh.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/abcd.R3D</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/abcd.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/A008_B009_1025IF_001.R3D</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/A008_B009_1025IF_001.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/d2 copy/efgh.R3D</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/d2 copy/efgh.mp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/abcd.R3D</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/abcd.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/A008_B009_1025IF_001.R3D</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/A008_B009_1025IF_001.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/d2 copy/efgh.R3D</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/d2 copy/efgh.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/abcd.R3D</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/abcd.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/abcd.R3D</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/abcd.mov</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
disable export button during processing
</commit_message>
<xml_diff>
--- a/conversion/conversion_log.xlsx
+++ b/conversion/conversion_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -673,6 +673,78 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/A008_B009_1025IF_001.R3D</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/A008_B009_1025IF_001.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/A008_B009_1025IF_001.R3D</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/A008_B009_1025IF_001.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/d2 copy/efgh.R3D</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/d2 copy/efgh.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/d2 copy/efgh.R3D</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/d2 copy/efgh.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/abcd.R3D</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/abcd.mov</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/A008_B009_1025IF_001.R3D</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/A008_B009_1025IF_001.mov</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
connecting to asset API
</commit_message>
<xml_diff>
--- a/conversion/conversion_log.xlsx
+++ b/conversion/conversion_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,6 +745,18 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1/A008_B009_1025IF.RDC/d2 copy/efgh.R3D</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>/Users/rayan/Downloads/d1_converted/A008_B009_1025IF.RDC/d2 copy/efgh.mov</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>